<commit_message>
Added voice output lines to the main nicla code. Optimised function and variables. Removed all instances of String datatype. Comments added to specific code.
</commit_message>
<xml_diff>
--- a/voice_lines/Voice Lines Table.xlsx
+++ b/voice_lines/Voice Lines Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cipri\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_Middlesex University\Third Year\PDE3400 Design Engineering Major Project\_GitHub\AURI_Smartwatch_Software\voice_lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96745606-74AA-44D9-BBC0-7A68F7F33526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9187741-2F9C-41A4-8BAC-388A71C368EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44040" yWindow="555" windowWidth="31365" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12105" yWindow="255" windowWidth="31350" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1028,6 +1028,16 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1055,16 +1065,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1347,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E164" sqref="B3:E164"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,8 +1362,8 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1374,12 +1374,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
@@ -2054,12 +2054,12 @@
       </c>
     </row>
     <row r="53" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="23"/>
-      <c r="C53" s="11" t="s">
+      <c r="B53" s="12"/>
+      <c r="C53" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="13"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="17"/>
     </row>
     <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="9" t="s">
@@ -2076,12 +2076,12 @@
       </c>
     </row>
     <row r="55" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="23"/>
-      <c r="C55" s="11" t="s">
+      <c r="B55" s="12"/>
+      <c r="C55" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="13"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="17"/>
     </row>
     <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="9" t="s">
@@ -2098,12 +2098,12 @@
       </c>
     </row>
     <row r="57" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="23"/>
-      <c r="C57" s="11" t="s">
+      <c r="B57" s="12"/>
+      <c r="C57" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="13"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="9" t="s">
@@ -2120,12 +2120,12 @@
       </c>
     </row>
     <row r="59" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="23"/>
-      <c r="C59" s="11" t="s">
+      <c r="B59" s="12"/>
+      <c r="C59" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="13"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="17"/>
     </row>
     <row r="60" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="9" t="s">
@@ -2198,12 +2198,12 @@
       </c>
     </row>
     <row r="65" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="23"/>
-      <c r="C65" s="11" t="s">
+      <c r="B65" s="12"/>
+      <c r="C65" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="13"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="17"/>
     </row>
     <row r="66" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="9" t="s">
@@ -2332,12 +2332,12 @@
       </c>
     </row>
     <row r="75" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="23"/>
-      <c r="C75" s="17" t="s">
+      <c r="B75" s="12"/>
+      <c r="C75" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="19"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="23"/>
     </row>
     <row r="76" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="9" t="s">
@@ -2438,12 +2438,12 @@
       </c>
     </row>
     <row r="83" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="23"/>
-      <c r="C83" s="17" t="s">
+      <c r="B83" s="12"/>
+      <c r="C83" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D83" s="18"/>
-      <c r="E83" s="19"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="23"/>
     </row>
     <row r="84" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="9" t="s">
@@ -2488,12 +2488,12 @@
       </c>
     </row>
     <row r="87" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="23"/>
-      <c r="C87" s="11" t="s">
+      <c r="B87" s="12"/>
+      <c r="C87" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D87" s="12"/>
-      <c r="E87" s="13"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="17"/>
     </row>
     <row r="88" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="9" t="s">
@@ -2580,12 +2580,12 @@
       </c>
     </row>
     <row r="94" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="23"/>
-      <c r="C94" s="11" t="s">
+      <c r="B94" s="12"/>
+      <c r="C94" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D94" s="12"/>
-      <c r="E94" s="13"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="17"/>
     </row>
     <row r="95" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="9" t="s">
@@ -2658,12 +2658,12 @@
       </c>
     </row>
     <row r="100" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="23"/>
-      <c r="C100" s="11" t="s">
+      <c r="B100" s="12"/>
+      <c r="C100" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D100" s="12"/>
-      <c r="E100" s="13"/>
+      <c r="D100" s="16"/>
+      <c r="E100" s="17"/>
     </row>
     <row r="101" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="9" t="s">
@@ -2680,12 +2680,12 @@
       </c>
     </row>
     <row r="102" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="23"/>
-      <c r="C102" s="14" t="s">
+      <c r="B102" s="12"/>
+      <c r="C102" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="D102" s="15"/>
-      <c r="E102" s="16"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="20"/>
     </row>
     <row r="103" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="9" t="s">
@@ -2842,12 +2842,12 @@
       </c>
     </row>
     <row r="114" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="23"/>
-      <c r="C114" s="14" t="s">
+      <c r="B114" s="12"/>
+      <c r="C114" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D114" s="15"/>
-      <c r="E114" s="16"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="20"/>
     </row>
     <row r="115" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="9" t="s">
@@ -2934,12 +2934,12 @@
       </c>
     </row>
     <row r="121" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="23"/>
-      <c r="C121" s="14" t="s">
+      <c r="B121" s="12"/>
+      <c r="C121" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D121" s="15"/>
-      <c r="E121" s="16"/>
+      <c r="D121" s="19"/>
+      <c r="E121" s="20"/>
     </row>
     <row r="122" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B122" s="9" t="s">
@@ -3180,12 +3180,12 @@
       </c>
     </row>
     <row r="139" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="23"/>
-      <c r="C139" s="11" t="s">
+      <c r="B139" s="12"/>
+      <c r="C139" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="D139" s="12"/>
-      <c r="E139" s="13"/>
+      <c r="D139" s="16"/>
+      <c r="E139" s="17"/>
     </row>
     <row r="140" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="9" t="s">
@@ -3202,12 +3202,12 @@
       </c>
     </row>
     <row r="141" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="23"/>
-      <c r="C141" s="11" t="s">
+      <c r="B141" s="12"/>
+      <c r="C141" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="D141" s="12"/>
-      <c r="E141" s="13"/>
+      <c r="D141" s="16"/>
+      <c r="E141" s="17"/>
     </row>
     <row r="142" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="9" t="s">
@@ -3224,12 +3224,12 @@
       </c>
     </row>
     <row r="143" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="23"/>
-      <c r="C143" s="11" t="s">
+      <c r="B143" s="12"/>
+      <c r="C143" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="D143" s="12"/>
-      <c r="E143" s="13"/>
+      <c r="D143" s="16"/>
+      <c r="E143" s="17"/>
     </row>
     <row r="144" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="9" t="s">
@@ -3260,12 +3260,12 @@
       </c>
     </row>
     <row r="146" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="23"/>
-      <c r="C146" s="11" t="s">
+      <c r="B146" s="12"/>
+      <c r="C146" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="D146" s="12"/>
-      <c r="E146" s="13"/>
+      <c r="D146" s="16"/>
+      <c r="E146" s="17"/>
     </row>
     <row r="147" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B147" s="9" t="s">
@@ -3282,12 +3282,12 @@
       </c>
     </row>
     <row r="148" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="23"/>
-      <c r="C148" s="11" t="s">
+      <c r="B148" s="12"/>
+      <c r="C148" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="D148" s="12"/>
-      <c r="E148" s="13"/>
+      <c r="D148" s="16"/>
+      <c r="E148" s="17"/>
     </row>
     <row r="149" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="9" t="s">
@@ -3304,12 +3304,12 @@
       </c>
     </row>
     <row r="150" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="23"/>
-      <c r="C150" s="11" t="s">
+      <c r="B150" s="12"/>
+      <c r="C150" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="D150" s="12"/>
-      <c r="E150" s="13"/>
+      <c r="D150" s="16"/>
+      <c r="E150" s="17"/>
     </row>
     <row r="151" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B151" s="9" t="s">
@@ -3452,12 +3452,12 @@
       </c>
     </row>
     <row r="161" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="23"/>
-      <c r="C161" s="11" t="s">
+      <c r="B161" s="12"/>
+      <c r="C161" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="D161" s="12"/>
-      <c r="E161" s="13"/>
+      <c r="D161" s="16"/>
+      <c r="E161" s="17"/>
     </row>
     <row r="162" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B162" s="9" t="s">
@@ -3474,12 +3474,12 @@
       </c>
     </row>
     <row r="163" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="23"/>
-      <c r="C163" s="11" t="s">
+      <c r="B163" s="12"/>
+      <c r="C163" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D163" s="12"/>
-      <c r="E163" s="13"/>
+      <c r="D163" s="16"/>
+      <c r="E163" s="17"/>
     </row>
     <row r="164" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B164" s="9" t="s">
@@ -3497,22 +3497,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="C139:E139"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C94:E94"/>
     <mergeCell ref="C161:E161"/>
     <mergeCell ref="C163:E163"/>
     <mergeCell ref="C141:E141"/>
@@ -3520,6 +3504,22 @@
     <mergeCell ref="C146:E146"/>
     <mergeCell ref="C148:E148"/>
     <mergeCell ref="C150:E150"/>
+    <mergeCell ref="C139:E139"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Optimised voice lines and file structure, while increasing audio quality and smoothness in DFPlayer playback. Implemented most features in the main code, only the caution outputs left. Added all comments.
</commit_message>
<xml_diff>
--- a/voice_lines/Voice Lines Table.xlsx
+++ b/voice_lines/Voice Lines Table.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_Middlesex University\Third Year\PDE3400 Design Engineering Major Project\_GitHub\AURI_Smartwatch_Software\voice_lines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cipri\Desktop\audio processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9187741-2F9C-41A4-8BAC-388A71C368EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0297183F-6E6D-4DD9-88EA-C2868F5F67F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12105" yWindow="255" windowWidth="31350" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="615" windowWidth="22245" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="275">
   <si>
     <t>FOLDER</t>
   </si>
@@ -54,9 +64,6 @@
     <t>003.wav</t>
   </si>
   <si>
-    <t>Meanwhile the humidity of your environment stands at</t>
-  </si>
-  <si>
     <t>004.wav</t>
   </si>
   <si>
@@ -117,18 +124,9 @@
     <t>In terms of the atmospheric pressure, it stands at:</t>
   </si>
   <si>
-    <t>Composed out of:</t>
-  </si>
-  <si>
     <t>Once converted to the sea-level pressure it is:</t>
   </si>
   <si>
-    <t>Dry air pressure.</t>
-  </si>
-  <si>
-    <t>Water vapor pressure, and:</t>
-  </si>
-  <si>
     <t xml:space="preserve">With a compass roll of: </t>
   </si>
   <si>
@@ -288,12 +286,6 @@
     <t>1% - 100%</t>
   </si>
   <si>
-    <t>001.wav - 251.wav</t>
-  </si>
-  <si>
-    <t>850 hectoPascals - 1100 hectoPascals</t>
-  </si>
-  <si>
     <t>CO2 OUTPUT</t>
   </si>
   <si>
@@ -582,9 +574,6 @@
     <t>001.wav - 151.wav</t>
   </si>
   <si>
-    <t>50 Beats Per Minute - 150 Beats per Minute</t>
-  </si>
-  <si>
     <t>HEART RATE OUTPUT</t>
   </si>
   <si>
@@ -663,30 +652,9 @@
     <t>If there is anything I can do for you, do ask</t>
   </si>
   <si>
-    <t>RAINFALL AMOUNT IN MM OUPUTS</t>
-  </si>
-  <si>
-    <t>ADVERT</t>
-  </si>
-  <si>
-    <t>0001.wav - 6000.wav</t>
-  </si>
-  <si>
-    <t>0.01 millimeters - 60 millimeters</t>
-  </si>
-  <si>
-    <t>MP3</t>
-  </si>
-  <si>
     <t>NUMBERS</t>
   </si>
   <si>
-    <t>0001.wav - 10001.wav</t>
-  </si>
-  <si>
-    <t>0 - 10000 number</t>
-  </si>
-  <si>
     <t>REGULAR FOLDER</t>
   </si>
   <si>
@@ -703,6 +671,195 @@
   </si>
   <si>
     <t>EAST</t>
+  </si>
+  <si>
+    <t>Meanwhile the humidity of your environment has been measured as:</t>
+  </si>
+  <si>
+    <t>001.wav - 101.wav</t>
+  </si>
+  <si>
+    <t>950 hectoPascals - 1050 hectoPascals</t>
+  </si>
+  <si>
+    <t>50 Beats Per Minute - 200 Beats per Minute</t>
+  </si>
+  <si>
+    <t>049.wav</t>
+  </si>
+  <si>
+    <t>050.wav</t>
+  </si>
+  <si>
+    <t>051.wav</t>
+  </si>
+  <si>
+    <t>053.wav</t>
+  </si>
+  <si>
+    <t>054.wav</t>
+  </si>
+  <si>
+    <t>055.wav</t>
+  </si>
+  <si>
+    <t>056.wav</t>
+  </si>
+  <si>
+    <t>057.wav</t>
+  </si>
+  <si>
+    <t>058.wav</t>
+  </si>
+  <si>
+    <t>059.wav</t>
+  </si>
+  <si>
+    <t>060.wav</t>
+  </si>
+  <si>
+    <t>The sensor needs to calibrate to the current environment before outputting an accurate gas resistance reading!</t>
+  </si>
+  <si>
+    <t>The Gas Resistance subsists at a level of</t>
+  </si>
+  <si>
+    <t>kilo-ohms</t>
+  </si>
+  <si>
+    <t>ohms</t>
+  </si>
+  <si>
+    <t>If I convert the temperature to Fahrenheit, it becomes</t>
+  </si>
+  <si>
+    <t>The battery is healthy and with no faults!</t>
+  </si>
+  <si>
+    <t>Attention! Faults regarding the battery have been detected!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The discomfort index is currently at </t>
+  </si>
+  <si>
+    <t>You spoke too quietly, or there was too much noise in your surroundings. PLEASE REPEAT THE COMMAND!</t>
+  </si>
+  <si>
+    <t>SOFTWARE ISSUE DETECTED. FAILED TO SETUP AUDIO SAMPLING</t>
+  </si>
+  <si>
+    <t>SOFTWARE OR HARDWARE ISSUE DETECTED. FAILED TO RECORD AUDIO</t>
+  </si>
+  <si>
+    <t>DEEP LEARNING ISSUE DETECTED. FAILED TO RUN THE CLASSIFIER</t>
+  </si>
+  <si>
+    <t>061.wav</t>
+  </si>
+  <si>
+    <t>062.wav</t>
+  </si>
+  <si>
+    <t>The saturation vapor pressure is equal to</t>
+  </si>
+  <si>
+    <t>The volume has been changed to:</t>
+  </si>
+  <si>
+    <t>And dry air pressure:</t>
+  </si>
+  <si>
+    <t>Composed out of water vapor pressure at:</t>
+  </si>
+  <si>
+    <t>The watch has not been setup. Please dock the watch and use the PC executable to sync the time and date!</t>
+  </si>
+  <si>
+    <t>001.wav - 999.wav</t>
+  </si>
+  <si>
+    <t>0 - 999 number</t>
+  </si>
+  <si>
+    <t>063.wav</t>
+  </si>
+  <si>
+    <t>Checking the system status. The BSEC sensor accuracy is at the level:</t>
+  </si>
+  <si>
+    <t>The battery voltage has been measured as:</t>
+  </si>
+  <si>
+    <t>The visible light has been identified as</t>
+  </si>
+  <si>
+    <t>Moreover, the infrared light is equal to</t>
+  </si>
+  <si>
+    <t>EXTRA VOICE LINES</t>
+  </si>
+  <si>
+    <t>In view of the weather classification, I can also forecast that there will be no rainfall</t>
+  </si>
+  <si>
+    <t>thousand</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>millimeters</t>
+  </si>
+  <si>
+    <t>millivolts</t>
+  </si>
+  <si>
+    <t>ohm</t>
+  </si>
+  <si>
+    <t>kilograms per cubic meter</t>
+  </si>
+  <si>
+    <t>grams of water vapor per cubic meter volume of air</t>
+  </si>
+  <si>
+    <t>A computed value higher than 35</t>
+  </si>
+  <si>
+    <t>0001.wav - 3500.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01 millimeters - 35 millimeters   </t>
+  </si>
+  <si>
+    <t>DECIMAL OUTPUT USED FOR ABSOLUTE HUMIDITY, RAINFALL FORECASTING AND AIR DENSITY</t>
+  </si>
+  <si>
+    <t>hundred</t>
+  </si>
+  <si>
+    <t>The Heat Index Condition cannot be calculated as the environment temperature is too low. Please consider the temperature as the absolute truth!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The estimated UV index based on the visible and infrared light is at the level of </t>
+  </si>
+  <si>
+    <t>The UV index is low. You can safely stay outside!</t>
+  </si>
+  <si>
+    <t>The UV index is moderate. Seek shade during midday hours! Try to wear sunscreen and a hat for protection!</t>
+  </si>
+  <si>
+    <t>The UV index is high. Seek shade during midday hours! Wear sunscreen and a hat for protection!</t>
+  </si>
+  <si>
+    <t>The UV index is very high. Avoid being outside during midday hours! It is a must to wear sunscreen, a shirt and a hat, for your protection!</t>
+  </si>
+  <si>
+    <t>The UV index is extreme. Must avoid being outside during midday hours! You need to wear sunscreen, a shirt and a hat, for your protection!</t>
+  </si>
+  <si>
+    <t>The density of the air has been calculated as:</t>
   </si>
 </sst>
 </file>
@@ -729,7 +886,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,6 +923,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -996,7 +1159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1032,19 +1195,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1054,15 +1229,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1345,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E164"/>
+  <dimension ref="B2:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E204" sqref="E204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1528,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="13"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1374,16 +1540,16 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
@@ -1397,7 +1563,7 @@
     </row>
     <row r="6" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
@@ -1411,7 +1577,7 @@
     </row>
     <row r="7" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
@@ -1425,1559 +1591,1571 @@
     </row>
     <row r="8" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C8" s="8">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C9" s="8">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>30</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C13" s="8">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>33</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>32</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C17" s="8">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C18" s="8">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C19" s="8">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C20" s="8">
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C21" s="8">
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C23" s="8">
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C24" s="8">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C25" s="8">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C26" s="8">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C27" s="8">
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C28" s="8">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C29" s="8">
         <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C30" s="8">
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C31" s="8">
         <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C33" s="8">
         <v>1</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C34" s="8">
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C35" s="8">
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C36" s="8">
         <v>1</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C37" s="8">
         <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C38" s="8">
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C39" s="8">
         <v>1</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C40" s="8">
         <v>1</v>
       </c>
       <c r="D40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C41" s="8">
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C42" s="8">
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C43" s="8">
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C44" s="8">
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C45" s="8">
         <v>1</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C46" s="8">
         <v>1</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C47" s="8">
         <v>1</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C48" s="8">
         <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C49" s="8">
         <v>1</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C50" s="8">
         <v>1</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C51" s="8">
         <v>1</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" s="8">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="8">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" s="8">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C55" s="8">
+        <v>1</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C56" s="8">
+        <v>1</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="8">
+        <v>1</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" s="8">
+        <v>1</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C52" s="8">
-        <v>1</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="12"/>
-      <c r="C53" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D53" s="16"/>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" s="10">
-        <v>2</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="12"/>
-      <c r="C55" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="D55" s="16"/>
-      <c r="E55" s="17"/>
-    </row>
-    <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C56" s="10">
-        <v>3</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="12"/>
-      <c r="C57" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="17"/>
-    </row>
-    <row r="58" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C58" s="10">
-        <v>4</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E58" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="12"/>
-      <c r="C59" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D59" s="16"/>
-      <c r="E59" s="17"/>
-    </row>
-    <row r="60" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C59" s="8">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C60" s="10">
-        <v>5</v>
+        <v>206</v>
+      </c>
+      <c r="C60" s="8">
+        <v>1</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C61" s="10">
-        <v>5</v>
+        <v>206</v>
+      </c>
+      <c r="C61" s="8">
+        <v>1</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C62" s="10">
-        <v>5</v>
+        <v>206</v>
+      </c>
+      <c r="C62" s="8">
+        <v>1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C63" s="10">
-        <v>5</v>
+        <v>206</v>
+      </c>
+      <c r="C63" s="8">
+        <v>1</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C64" s="10">
-        <v>5</v>
+        <v>206</v>
+      </c>
+      <c r="C64" s="8">
+        <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="12"/>
-      <c r="C65" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="17"/>
+        <v>226</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C65" s="8">
+        <v>1</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="66" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C66" s="10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>3</v>
+        <v>240</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>91</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C67" s="10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>4</v>
+        <v>248</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>90</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C68" s="10">
-        <v>6</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="17"/>
     </row>
     <row r="69" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C69" s="10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C70" s="10">
-        <v>6</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>94</v>
-      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D70" s="16"/>
+      <c r="E70" s="17"/>
     </row>
     <row r="71" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C71" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C72" s="10">
-        <v>6</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="B72" s="13"/>
+      <c r="C72" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="17"/>
     </row>
     <row r="73" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C73" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>15</v>
+        <v>213</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>97</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C74" s="10">
-        <v>6</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="B74" s="12"/>
+      <c r="C74" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D74" s="16"/>
+      <c r="E74" s="17"/>
     </row>
     <row r="75" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="12"/>
-      <c r="C75" s="21" t="s">
+      <c r="B75" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C75" s="10">
+        <v>5</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D75" s="22"/>
-      <c r="E75" s="23"/>
     </row>
     <row r="76" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C76" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C77" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C78" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>101</v>
+        <v>9</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C79" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="E79" s="7" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="80" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C80" s="10">
-        <v>7</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="B80" s="12"/>
+      <c r="C80" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D80" s="16"/>
+      <c r="E80" s="17"/>
     </row>
     <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C81" s="10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C82" s="10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="12"/>
-      <c r="C83" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D83" s="22"/>
-      <c r="E83" s="23"/>
+      <c r="B83" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C83" s="10">
+        <v>6</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="84" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C84" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C85" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C86" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="12"/>
-      <c r="C87" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D87" s="16"/>
-      <c r="E87" s="17"/>
+      <c r="B87" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C87" s="10">
+        <v>6</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="88" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C88" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C89" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C90" s="10">
-        <v>8</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="B90" s="12"/>
+      <c r="C90" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" s="20"/>
+      <c r="E90" s="21"/>
     </row>
     <row r="91" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C91" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C92" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C93" s="10">
+        <v>7</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E93" s="6" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="12"/>
-      <c r="C94" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="D94" s="16"/>
-      <c r="E94" s="17"/>
+      <c r="B94" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C94" s="10">
+        <v>7</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="95" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C95" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C96" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C97" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C98" s="10">
-        <v>8</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>126</v>
-      </c>
+      <c r="B98" s="12"/>
+      <c r="C98" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D98" s="20"/>
+      <c r="E98" s="21"/>
     </row>
     <row r="99" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C99" s="10">
         <v>8</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="12"/>
-      <c r="C100" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D100" s="16"/>
-      <c r="E100" s="17"/>
+      <c r="B100" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C100" s="10">
+        <v>8</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="101" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="9" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="C101" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="12"/>
       <c r="C102" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D102" s="19"/>
-      <c r="E102" s="20"/>
-    </row>
-    <row r="103" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="D102" s="16"/>
+      <c r="E102" s="17"/>
+    </row>
+    <row r="103" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C103" s="10">
-        <v>10</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>167</v>
+        <v>112</v>
       </c>
     </row>
     <row r="104" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C104" s="10">
+        <v>8</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E104" s="6" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
     </row>
     <row r="105" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C105" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>169</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C106" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>170</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C107" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
     </row>
     <row r="108" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C108" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>173</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C109" s="10">
-        <v>10</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>172</v>
-      </c>
+      <c r="B109" s="12"/>
+      <c r="C109" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D109" s="16"/>
+      <c r="E109" s="17"/>
     </row>
     <row r="110" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C110" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
     </row>
     <row r="111" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C111" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C112" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>176</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C113" s="10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>177</v>
+        <v>120</v>
       </c>
     </row>
     <row r="114" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="12"/>
-      <c r="C114" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D114" s="19"/>
-      <c r="E114" s="20"/>
-    </row>
-    <row r="115" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C115" s="10">
-        <v>11</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>178</v>
-      </c>
+      <c r="B114" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C114" s="10">
+        <v>8</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="12"/>
+      <c r="C115" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D115" s="16"/>
+      <c r="E115" s="17"/>
     </row>
     <row r="116" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="9" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="C116" s="10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
     </row>
     <row r="117" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C117" s="10">
-        <v>11</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B117" s="12"/>
+      <c r="C117" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D117" s="23"/>
+      <c r="E117" s="24"/>
+    </row>
+    <row r="118" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C118" s="10">
-        <v>11</v>
-      </c>
-      <c r="D118" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D118" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E118" s="6" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="119" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B119" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C119" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="120" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B120" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C120" s="10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="121" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="12"/>
-      <c r="C121" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D121" s="19"/>
-      <c r="E121" s="20"/>
-    </row>
-    <row r="122" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C121" s="10">
+        <v>10</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B122" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C122" s="10">
-        <v>12</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
     </row>
     <row r="123" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C123" s="10">
+        <v>10</v>
+      </c>
+      <c r="D123" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E123" s="6" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
     <row r="124" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C124" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>166</v>
@@ -2985,541 +3163,1042 @@
     </row>
     <row r="125" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C125" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="126" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C126" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>225</v>
+        <v>169</v>
       </c>
     </row>
     <row r="127" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C127" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="128" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C128" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="129" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C129" s="10">
-        <v>12</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E129" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B129" s="12"/>
+      <c r="C129" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D129" s="23"/>
+      <c r="E129" s="24"/>
+    </row>
+    <row r="130" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C130" s="10">
-        <v>12</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="131" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C131" s="10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="132" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B132" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C132" s="10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="133" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B133" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C133" s="10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
     </row>
     <row r="134" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C134" s="10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="135" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B135" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C135" s="10">
+        <v>11</v>
+      </c>
+      <c r="D135" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D135" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="E135" s="6" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
     </row>
     <row r="136" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C136" s="10">
-        <v>12</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E136" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B136" s="12"/>
+      <c r="C136" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D136" s="23"/>
+      <c r="E136" s="24"/>
+    </row>
+    <row r="137" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C137" s="10">
         <v>12</v>
       </c>
-      <c r="D137" s="3" t="s">
-        <v>23</v>
+      <c r="D137" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="138" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C138" s="10">
         <v>12</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="139" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="12"/>
-      <c r="C139" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D139" s="16"/>
-      <c r="E139" s="17"/>
+      <c r="B139" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C139" s="10">
+        <v>12</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="140" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C140" s="10">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>184</v>
+        <v>9</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
     </row>
     <row r="141" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="12"/>
-      <c r="C141" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D141" s="16"/>
-      <c r="E141" s="17"/>
+      <c r="B141" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C141" s="10">
+        <v>12</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="142" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C142" s="10">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>187</v>
+        <v>12</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
     </row>
     <row r="143" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="12"/>
-      <c r="C143" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D143" s="16"/>
-      <c r="E143" s="17"/>
+      <c r="B143" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C143" s="10">
+        <v>12</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="144" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C144" s="10">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>191</v>
+        <v>14</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
     </row>
     <row r="145" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C145" s="10">
+        <v>12</v>
+      </c>
+      <c r="D145" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D145" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E145" s="6" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
     </row>
     <row r="146" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="12"/>
-      <c r="C146" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="D146" s="16"/>
-      <c r="E146" s="17"/>
+      <c r="B146" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C146" s="10">
+        <v>12</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="147" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B147" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C147" s="10">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>195</v>
+        <v>17</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
     </row>
     <row r="148" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="12"/>
-      <c r="C148" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="D148" s="16"/>
-      <c r="E148" s="17"/>
+      <c r="B148" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C148" s="10">
+        <v>12</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="149" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C149" s="10">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>199</v>
+        <v>19</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
     </row>
     <row r="150" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="12"/>
-      <c r="C150" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="D150" s="16"/>
-      <c r="E150" s="17"/>
+      <c r="B150" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C150" s="10">
+        <v>12</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E150" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="151" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B151" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C151" s="10">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B152" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C152" s="10">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>203</v>
+        <v>149</v>
       </c>
     </row>
     <row r="153" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C153" s="10">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>204</v>
+        <v>146</v>
       </c>
     </row>
     <row r="154" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C154" s="10">
-        <v>18</v>
-      </c>
-      <c r="D154" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E154" s="6" t="s">
-        <v>205</v>
-      </c>
+      <c r="B154" s="12"/>
+      <c r="C154" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D154" s="16"/>
+      <c r="E154" s="17"/>
     </row>
     <row r="155" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C155" s="10">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
     </row>
     <row r="156" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C156" s="10">
-        <v>18</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E156" s="6" t="s">
-        <v>207</v>
-      </c>
+      <c r="B156" s="12"/>
+      <c r="C156" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="D156" s="16"/>
+      <c r="E156" s="17"/>
     </row>
     <row r="157" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C157" s="10">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>14</v>
+        <v>180</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
     </row>
     <row r="158" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C158" s="10">
-        <v>18</v>
-      </c>
-      <c r="D158" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E158" s="6" t="s">
-        <v>209</v>
-      </c>
+      <c r="B158" s="12"/>
+      <c r="C158" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D158" s="16"/>
+      <c r="E158" s="17"/>
     </row>
     <row r="159" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B159" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C159" s="10">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>16</v>
+        <v>184</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
     </row>
     <row r="160" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B160" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C160" s="10">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
     </row>
     <row r="161" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B161" s="12"/>
-      <c r="C161" s="15" t="s">
-        <v>212</v>
+      <c r="C161" s="18" t="s">
+        <v>190</v>
       </c>
       <c r="D161" s="16"/>
       <c r="E161" s="17"/>
     </row>
     <row r="162" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B162" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C162" s="10" t="s">
-        <v>213</v>
+        <v>206</v>
+      </c>
+      <c r="C162" s="10">
+        <v>16</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>215</v>
+        <v>189</v>
       </c>
     </row>
     <row r="163" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B163" s="12"/>
-      <c r="C163" s="15" t="s">
-        <v>217</v>
+      <c r="C163" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="D163" s="16"/>
       <c r="E163" s="17"/>
     </row>
     <row r="164" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B164" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C164" s="10" t="s">
-        <v>216</v>
+        <v>206</v>
+      </c>
+      <c r="C164" s="10">
+        <v>17</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>219</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="12"/>
+      <c r="C165" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D165" s="16"/>
+      <c r="E165" s="17"/>
+    </row>
+    <row r="166" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C166" s="10">
+        <v>18</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E166" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B167" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C167" s="10">
+        <v>18</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E167" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C168" s="10">
+        <v>18</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E168" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="169" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B169" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C169" s="10">
+        <v>18</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E169" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="170" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C170" s="10">
+        <v>18</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E170" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="171" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B171" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C171" s="10">
+        <v>18</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E171" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="172" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C172" s="10">
+        <v>18</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E172" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="173" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B173" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C173" s="10">
+        <v>18</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E173" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="174" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C174" s="10">
+        <v>18</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="175" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B175" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C175" s="10">
+        <v>18</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E175" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="176" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B176" s="12"/>
+      <c r="C176" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D176" s="16"/>
+      <c r="E176" s="17"/>
+    </row>
+    <row r="177" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B177" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C177" s="10">
+        <v>19</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E177" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B178" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C178" s="10">
+        <v>19</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E178" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="179" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B179" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C179" s="10">
+        <v>19</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E179" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="180" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C180" s="10">
+        <v>19</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E180" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="181" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B181" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C181" s="10">
+        <v>19</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E181" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="182" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C182" s="10">
+        <v>19</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E182" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="183" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C183" s="10">
+        <v>19</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E183" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="184" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C184" s="10">
+        <v>19</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E184" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="185" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C185" s="10">
+        <v>19</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="186" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B186" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C186" s="10">
+        <v>19</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="187" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B187" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C187" s="10">
+        <v>19</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E187" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="188" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B188" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C188" s="10">
+        <v>19</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E188" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="189" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B189" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C189" s="10">
+        <v>19</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E189" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="190" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C190" s="10">
+        <v>19</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E190" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="191" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B191" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C191" s="10">
+        <v>19</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E191" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="192" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C192" s="10">
+        <v>19</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E192" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="193" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C193" s="10">
+        <v>19</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E193" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="194" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C194" s="10">
+        <v>19</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E194" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="195" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B195" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C195" s="10">
+        <v>19</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E195" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="196" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C196" s="10">
+        <v>19</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E196" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="197" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B197" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C197" s="10">
+        <v>19</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E197" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="198" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B198" s="12"/>
+      <c r="C198" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D198" s="16"/>
+      <c r="E198" s="17"/>
+    </row>
+    <row r="199" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B199" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C199" s="10">
+        <v>20</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E199" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="200" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="12"/>
+      <c r="C200" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D200" s="16"/>
+      <c r="E200" s="17"/>
+    </row>
+    <row r="201" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B201" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C201" s="10">
+        <v>21</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E201" s="6" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="C200:E200"/>
+    <mergeCell ref="C154:E154"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="C136:E136"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C156:E156"/>
+    <mergeCell ref="C158:E158"/>
     <mergeCell ref="C161:E161"/>
     <mergeCell ref="C163:E163"/>
-    <mergeCell ref="C141:E141"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="C146:E146"/>
-    <mergeCell ref="C148:E148"/>
-    <mergeCell ref="C150:E150"/>
-    <mergeCell ref="C139:E139"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C165:E165"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C68:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added environment checks for adverse health effects. Added extra comments.
</commit_message>
<xml_diff>
--- a/voice_lines/Voice Lines Table.xlsx
+++ b/voice_lines/Voice Lines Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cipri\Desktop\audio processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0297183F-6E6D-4DD9-88EA-C2868F5F67F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2087ED14-F310-484A-B26D-D2F26D275AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="615" windowWidth="22245" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41265" yWindow="1980" windowWidth="22245" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="281">
   <si>
     <t>FOLDER</t>
   </si>
@@ -860,6 +860,24 @@
   </si>
   <si>
     <t>The density of the air has been calculated as:</t>
+  </si>
+  <si>
+    <t>COMPUTING VOICE LINES (AFTER THE VOICE COMMAND SPOKEN BY THE USER)</t>
+  </si>
+  <si>
+    <t>Cyphering</t>
+  </si>
+  <si>
+    <t>Assessing</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t>Computing</t>
+  </si>
+  <si>
+    <t>Evaluating</t>
   </si>
 </sst>
 </file>
@@ -1511,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E201"/>
+  <dimension ref="B2:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E204" sqref="E204"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E214" sqref="E214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4132,50 +4150,128 @@
     <row r="198" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B198" s="12"/>
       <c r="C198" s="18" t="s">
-        <v>205</v>
+        <v>275</v>
       </c>
       <c r="D198" s="16"/>
       <c r="E198" s="17"/>
     </row>
     <row r="199" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B199" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C199" s="10">
         <v>20</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
     </row>
     <row r="200" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="12"/>
-      <c r="C200" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="D200" s="16"/>
-      <c r="E200" s="17"/>
+      <c r="B200" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C200" s="10">
+        <v>20</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E200" s="6" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="201" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B201" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C201" s="10">
+        <v>20</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E201" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="202" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B202" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C202" s="10">
+        <v>20</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E202" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="203" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B203" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C203" s="10">
+        <v>20</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E203" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="204" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B204" s="12"/>
+      <c r="C204" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D204" s="16"/>
+      <c r="E204" s="17"/>
+    </row>
+    <row r="205" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B205" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C205" s="10">
+        <v>20</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E205" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="206" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B206" s="12"/>
+      <c r="C206" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D206" s="16"/>
+      <c r="E206" s="17"/>
+    </row>
+    <row r="207" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B207" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C201" s="10">
+      <c r="C207" s="10">
         <v>21</v>
       </c>
-      <c r="D201" s="3" t="s">
+      <c r="D207" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E201" s="6" t="s">
+      <c r="E207" s="6" t="s">
         <v>264</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="C200:E200"/>
+  <mergeCells count="25">
+    <mergeCell ref="C206:E206"/>
     <mergeCell ref="C154:E154"/>
     <mergeCell ref="C80:E80"/>
     <mergeCell ref="C90:E90"/>
@@ -4187,9 +4283,10 @@
     <mergeCell ref="C129:E129"/>
     <mergeCell ref="C115:E115"/>
     <mergeCell ref="C176:E176"/>
+    <mergeCell ref="C198:E198"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C204:E204"/>
     <mergeCell ref="C156:E156"/>
     <mergeCell ref="C158:E158"/>
     <mergeCell ref="C161:E161"/>

</xml_diff>

<commit_message>
Added some new voice lines for sensor checks. Added new voice lines for when the volume is at the lowest/highest. Added all environmental checks. Added all comments to both Nicla and Xiao code. Added 2 extra voice commands to be recognised.
</commit_message>
<xml_diff>
--- a/voice_lines/Voice Lines Table.xlsx
+++ b/voice_lines/Voice Lines Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cipri\Desktop\audio processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2087ED14-F310-484A-B26D-D2F26D275AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8849205-3845-48AD-BFAE-8D8820EA79F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41265" yWindow="1980" windowWidth="22245" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40635" yWindow="1680" windowWidth="35520" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="284">
   <si>
     <t>FOLDER</t>
   </si>
@@ -878,6 +878,15 @@
   </si>
   <si>
     <t>Evaluating</t>
+  </si>
+  <si>
+    <t>Volume is at the lowest level of 5! It cannot be decreased further!</t>
+  </si>
+  <si>
+    <t>Volume is at the highest level of 30! It cannot be increased further!</t>
+  </si>
+  <si>
+    <t>The battery level is VERY LOW. Please dock the watch as soon as possible!</t>
   </si>
 </sst>
 </file>
@@ -1216,19 +1225,13 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1248,6 +1251,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1529,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E207"/>
+  <dimension ref="B2:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E214" sqref="E214"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D200" sqref="D200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1555,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1558,12 +1567,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
-      <c r="C4" s="16" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
@@ -2449,11 +2458,11 @@
     </row>
     <row r="68" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="13"/>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="17"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="16"/>
     </row>
     <row r="69" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="9" t="s">
@@ -2471,11 +2480,11 @@
     </row>
     <row r="70" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="13"/>
-      <c r="C70" s="16" t="s">
+      <c r="C70" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D70" s="16"/>
-      <c r="E70" s="17"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="16"/>
     </row>
     <row r="71" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="9" t="s">
@@ -2493,11 +2502,11 @@
     </row>
     <row r="72" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="13"/>
-      <c r="C72" s="16" t="s">
+      <c r="C72" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="17"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="16"/>
     </row>
     <row r="73" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="9" t="s">
@@ -2515,11 +2524,11 @@
     </row>
     <row r="74" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="12"/>
-      <c r="C74" s="18" t="s">
+      <c r="C74" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D74" s="16"/>
-      <c r="E74" s="17"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="16"/>
     </row>
     <row r="75" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="9" t="s">
@@ -2593,11 +2602,11 @@
     </row>
     <row r="80" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="12"/>
-      <c r="C80" s="18" t="s">
+      <c r="C80" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="16"/>
-      <c r="E80" s="17"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="16"/>
     </row>
     <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="9" t="s">
@@ -2727,11 +2736,11 @@
     </row>
     <row r="90" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="12"/>
-      <c r="C90" s="19" t="s">
+      <c r="C90" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="D90" s="20"/>
-      <c r="E90" s="21"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19"/>
     </row>
     <row r="91" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="9" t="s">
@@ -2833,11 +2842,11 @@
     </row>
     <row r="98" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="12"/>
-      <c r="C98" s="19" t="s">
+      <c r="C98" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="D98" s="20"/>
-      <c r="E98" s="21"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="19"/>
     </row>
     <row r="99" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="9" t="s">
@@ -2883,11 +2892,11 @@
     </row>
     <row r="102" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="12"/>
-      <c r="C102" s="18" t="s">
+      <c r="C102" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D102" s="16"/>
-      <c r="E102" s="17"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="16"/>
     </row>
     <row r="103" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="9" t="s">
@@ -2975,11 +2984,11 @@
     </row>
     <row r="109" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="12"/>
-      <c r="C109" s="18" t="s">
+      <c r="C109" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D109" s="16"/>
-      <c r="E109" s="17"/>
+      <c r="D109" s="15"/>
+      <c r="E109" s="16"/>
     </row>
     <row r="110" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="9" t="s">
@@ -3053,11 +3062,11 @@
     </row>
     <row r="115" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="12"/>
-      <c r="C115" s="18" t="s">
+      <c r="C115" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D115" s="16"/>
-      <c r="E115" s="17"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="16"/>
     </row>
     <row r="116" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="9" t="s">
@@ -3075,11 +3084,11 @@
     </row>
     <row r="117" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="12"/>
-      <c r="C117" s="22" t="s">
+      <c r="C117" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="D117" s="23"/>
-      <c r="E117" s="24"/>
+      <c r="D117" s="21"/>
+      <c r="E117" s="22"/>
     </row>
     <row r="118" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="9" t="s">
@@ -3237,11 +3246,11 @@
     </row>
     <row r="129" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="12"/>
-      <c r="C129" s="22" t="s">
+      <c r="C129" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="D129" s="23"/>
-      <c r="E129" s="24"/>
+      <c r="D129" s="21"/>
+      <c r="E129" s="22"/>
     </row>
     <row r="130" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="9" t="s">
@@ -3329,11 +3338,11 @@
     </row>
     <row r="136" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="12"/>
-      <c r="C136" s="22" t="s">
+      <c r="C136" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="D136" s="23"/>
-      <c r="E136" s="24"/>
+      <c r="D136" s="21"/>
+      <c r="E136" s="22"/>
     </row>
     <row r="137" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="9" t="s">
@@ -3575,11 +3584,11 @@
     </row>
     <row r="154" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B154" s="12"/>
-      <c r="C154" s="18" t="s">
+      <c r="C154" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="D154" s="16"/>
-      <c r="E154" s="17"/>
+      <c r="D154" s="15"/>
+      <c r="E154" s="16"/>
     </row>
     <row r="155" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="9" t="s">
@@ -3597,11 +3606,11 @@
     </row>
     <row r="156" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="12"/>
-      <c r="C156" s="18" t="s">
+      <c r="C156" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D156" s="16"/>
-      <c r="E156" s="17"/>
+      <c r="D156" s="15"/>
+      <c r="E156" s="16"/>
     </row>
     <row r="157" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="9" t="s">
@@ -3619,11 +3628,11 @@
     </row>
     <row r="158" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="12"/>
-      <c r="C158" s="18" t="s">
+      <c r="C158" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D158" s="16"/>
-      <c r="E158" s="17"/>
+      <c r="D158" s="15"/>
+      <c r="E158" s="16"/>
     </row>
     <row r="159" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B159" s="9" t="s">
@@ -3655,11 +3664,11 @@
     </row>
     <row r="161" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B161" s="12"/>
-      <c r="C161" s="18" t="s">
+      <c r="C161" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="D161" s="16"/>
-      <c r="E161" s="17"/>
+      <c r="D161" s="15"/>
+      <c r="E161" s="16"/>
     </row>
     <row r="162" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B162" s="9" t="s">
@@ -3677,11 +3686,11 @@
     </row>
     <row r="163" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B163" s="12"/>
-      <c r="C163" s="18" t="s">
+      <c r="C163" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="D163" s="16"/>
-      <c r="E163" s="17"/>
+      <c r="D163" s="15"/>
+      <c r="E163" s="16"/>
     </row>
     <row r="164" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B164" s="9" t="s">
@@ -3699,11 +3708,11 @@
     </row>
     <row r="165" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B165" s="12"/>
-      <c r="C165" s="18" t="s">
+      <c r="C165" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="D165" s="16"/>
-      <c r="E165" s="17"/>
+      <c r="D165" s="15"/>
+      <c r="E165" s="16"/>
     </row>
     <row r="166" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B166" s="9" t="s">
@@ -3847,11 +3856,11 @@
     </row>
     <row r="176" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B176" s="12"/>
-      <c r="C176" s="18" t="s">
+      <c r="C176" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="D176" s="16"/>
-      <c r="E176" s="17"/>
+      <c r="D176" s="15"/>
+      <c r="E176" s="16"/>
     </row>
     <row r="177" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B177" s="9" t="s">
@@ -4148,25 +4157,31 @@
       </c>
     </row>
     <row r="198" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B198" s="12"/>
-      <c r="C198" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="D198" s="16"/>
-      <c r="E198" s="17"/>
+      <c r="B198" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C198" s="10">
+        <v>19</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E198" s="6" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="199" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B199" s="9" t="s">
         <v>206</v>
       </c>
       <c r="C199" s="10">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="200" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4174,28 +4189,22 @@
         <v>206</v>
       </c>
       <c r="C200" s="10">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="201" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C201" s="10">
-        <v>20</v>
-      </c>
-      <c r="D201" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E201" s="6" t="s">
-        <v>280</v>
-      </c>
+      <c r="B201" s="12"/>
+      <c r="C201" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="D201" s="15"/>
+      <c r="E201" s="16"/>
     </row>
     <row r="202" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B202" s="9" t="s">
@@ -4205,10 +4214,10 @@
         <v>20</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="203" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4219,59 +4228,113 @@
         <v>20</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="204" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="12"/>
-      <c r="C204" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="D204" s="16"/>
-      <c r="E204" s="17"/>
+      <c r="B204" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C204" s="10">
+        <v>20</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E204" s="6" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="205" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B205" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C205" s="10">
         <v>20</v>
       </c>
       <c r="D205" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E205" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="206" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B206" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C206" s="10">
+        <v>20</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E206" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="207" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B207" s="12"/>
+      <c r="C207" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D207" s="15"/>
+      <c r="E207" s="16"/>
+    </row>
+    <row r="208" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B208" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C208" s="10">
+        <v>20</v>
+      </c>
+      <c r="D208" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E205" s="6" t="s">
+      <c r="E208" s="6" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="206" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B206" s="12"/>
-      <c r="C206" s="18" t="s">
+    <row r="209" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B209" s="12"/>
+      <c r="C209" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="D206" s="16"/>
-      <c r="E206" s="17"/>
-    </row>
-    <row r="207" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B207" s="9" t="s">
+      <c r="D209" s="15"/>
+      <c r="E209" s="16"/>
+    </row>
+    <row r="210" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B210" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C207" s="10">
+      <c r="C210" s="10">
         <v>21</v>
       </c>
-      <c r="D207" s="3" t="s">
+      <c r="D210" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E207" s="6" t="s">
+      <c r="E210" s="6" t="s">
         <v>264</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C206:E206"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C156:E156"/>
+    <mergeCell ref="C158:E158"/>
+    <mergeCell ref="C161:E161"/>
+    <mergeCell ref="C163:E163"/>
+    <mergeCell ref="C165:E165"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C209:E209"/>
     <mergeCell ref="C154:E154"/>
     <mergeCell ref="C80:E80"/>
     <mergeCell ref="C90:E90"/>
@@ -4283,19 +4346,7 @@
     <mergeCell ref="C129:E129"/>
     <mergeCell ref="C115:E115"/>
     <mergeCell ref="C176:E176"/>
-    <mergeCell ref="C198:E198"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="C156:E156"/>
-    <mergeCell ref="C158:E158"/>
-    <mergeCell ref="C161:E161"/>
-    <mergeCell ref="C163:E163"/>
-    <mergeCell ref="C165:E165"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C201:E201"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Upgraded everything. Fixed many bugs, implemented proper environment checks. Added extra outputs.
</commit_message>
<xml_diff>
--- a/voice_lines/Voice Lines Table.xlsx
+++ b/voice_lines/Voice Lines Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cipri\Desktop\audio processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_Middlesex University\Third Year\PDE3400 Design Engineering Major Project\Development\audio processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8849205-3845-48AD-BFAE-8D8820EA79F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B5C685-510D-4745-B906-3B821A5A301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40635" yWindow="1680" windowWidth="35520" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48225" yWindow="1425" windowWidth="25605" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="293">
   <si>
     <t>FOLDER</t>
   </si>
@@ -887,6 +887,33 @@
   </si>
   <si>
     <t>The battery level is VERY LOW. Please dock the watch as soon as possible!</t>
+  </si>
+  <si>
+    <t>QUATERNION ANGLES</t>
+  </si>
+  <si>
+    <t>The gravity vector quaternion values are as follows</t>
+  </si>
+  <si>
+    <t>Meanwhile, the geomagnetic rotation vector has the following coordinates</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>EXTRA HEART RATE</t>
+  </si>
+  <si>
+    <t>The heart rate is over 120BPM!</t>
   </si>
 </sst>
 </file>
@@ -1225,13 +1252,19 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1251,12 +1284,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1538,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E210"/>
+  <dimension ref="B2:E219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D200" sqref="D200"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,7 +1582,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="23"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1567,12 +1594,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="24"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
@@ -2458,11 +2485,11 @@
     </row>
     <row r="68" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="13"/>
-      <c r="C68" s="15" t="s">
+      <c r="C68" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="D68" s="15"/>
-      <c r="E68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="17"/>
     </row>
     <row r="69" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="9" t="s">
@@ -2480,11 +2507,11 @@
     </row>
     <row r="70" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="13"/>
-      <c r="C70" s="15" t="s">
+      <c r="C70" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D70" s="15"/>
-      <c r="E70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="17"/>
     </row>
     <row r="71" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="9" t="s">
@@ -2502,11 +2529,11 @@
     </row>
     <row r="72" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="13"/>
-      <c r="C72" s="15" t="s">
+      <c r="C72" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D72" s="15"/>
-      <c r="E72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="17"/>
     </row>
     <row r="73" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="9" t="s">
@@ -2524,11 +2551,11 @@
     </row>
     <row r="74" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="12"/>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D74" s="15"/>
-      <c r="E74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="17"/>
     </row>
     <row r="75" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="9" t="s">
@@ -2602,11 +2629,11 @@
     </row>
     <row r="80" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="12"/>
-      <c r="C80" s="14" t="s">
+      <c r="C80" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="15"/>
-      <c r="E80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="17"/>
     </row>
     <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="9" t="s">
@@ -2736,11 +2763,11 @@
     </row>
     <row r="90" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="12"/>
-      <c r="C90" s="17" t="s">
+      <c r="C90" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D90" s="18"/>
-      <c r="E90" s="19"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="21"/>
     </row>
     <row r="91" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="9" t="s">
@@ -2842,11 +2869,11 @@
     </row>
     <row r="98" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="12"/>
-      <c r="C98" s="17" t="s">
+      <c r="C98" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D98" s="18"/>
-      <c r="E98" s="19"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="21"/>
     </row>
     <row r="99" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="9" t="s">
@@ -2892,11 +2919,11 @@
     </row>
     <row r="102" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="12"/>
-      <c r="C102" s="14" t="s">
+      <c r="C102" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D102" s="15"/>
-      <c r="E102" s="16"/>
+      <c r="D102" s="16"/>
+      <c r="E102" s="17"/>
     </row>
     <row r="103" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="9" t="s">
@@ -2984,11 +3011,11 @@
     </row>
     <row r="109" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="12"/>
-      <c r="C109" s="14" t="s">
+      <c r="C109" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D109" s="15"/>
-      <c r="E109" s="16"/>
+      <c r="D109" s="16"/>
+      <c r="E109" s="17"/>
     </row>
     <row r="110" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="9" t="s">
@@ -3062,11 +3089,11 @@
     </row>
     <row r="115" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="12"/>
-      <c r="C115" s="14" t="s">
+      <c r="C115" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D115" s="15"/>
-      <c r="E115" s="16"/>
+      <c r="D115" s="16"/>
+      <c r="E115" s="17"/>
     </row>
     <row r="116" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="9" t="s">
@@ -3084,11 +3111,11 @@
     </row>
     <row r="117" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="12"/>
-      <c r="C117" s="20" t="s">
+      <c r="C117" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D117" s="21"/>
-      <c r="E117" s="22"/>
+      <c r="D117" s="23"/>
+      <c r="E117" s="24"/>
     </row>
     <row r="118" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="9" t="s">
@@ -3246,11 +3273,11 @@
     </row>
     <row r="129" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="12"/>
-      <c r="C129" s="20" t="s">
+      <c r="C129" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D129" s="21"/>
-      <c r="E129" s="22"/>
+      <c r="D129" s="23"/>
+      <c r="E129" s="24"/>
     </row>
     <row r="130" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="9" t="s">
@@ -3338,11 +3365,11 @@
     </row>
     <row r="136" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="12"/>
-      <c r="C136" s="20" t="s">
+      <c r="C136" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D136" s="21"/>
-      <c r="E136" s="22"/>
+      <c r="D136" s="23"/>
+      <c r="E136" s="24"/>
     </row>
     <row r="137" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="9" t="s">
@@ -3584,11 +3611,11 @@
     </row>
     <row r="154" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B154" s="12"/>
-      <c r="C154" s="14" t="s">
+      <c r="C154" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="D154" s="15"/>
-      <c r="E154" s="16"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="17"/>
     </row>
     <row r="155" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="9" t="s">
@@ -3606,11 +3633,11 @@
     </row>
     <row r="156" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="12"/>
-      <c r="C156" s="14" t="s">
+      <c r="C156" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="D156" s="15"/>
-      <c r="E156" s="16"/>
+      <c r="D156" s="16"/>
+      <c r="E156" s="17"/>
     </row>
     <row r="157" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="9" t="s">
@@ -3628,11 +3655,11 @@
     </row>
     <row r="158" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="12"/>
-      <c r="C158" s="14" t="s">
+      <c r="C158" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="D158" s="15"/>
-      <c r="E158" s="16"/>
+      <c r="D158" s="16"/>
+      <c r="E158" s="17"/>
     </row>
     <row r="159" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B159" s="9" t="s">
@@ -3664,11 +3691,11 @@
     </row>
     <row r="161" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B161" s="12"/>
-      <c r="C161" s="14" t="s">
+      <c r="C161" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="D161" s="15"/>
-      <c r="E161" s="16"/>
+      <c r="D161" s="16"/>
+      <c r="E161" s="17"/>
     </row>
     <row r="162" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B162" s="9" t="s">
@@ -3686,11 +3713,11 @@
     </row>
     <row r="163" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B163" s="12"/>
-      <c r="C163" s="14" t="s">
+      <c r="C163" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="D163" s="15"/>
-      <c r="E163" s="16"/>
+      <c r="D163" s="16"/>
+      <c r="E163" s="17"/>
     </row>
     <row r="164" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B164" s="9" t="s">
@@ -3708,11 +3735,11 @@
     </row>
     <row r="165" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B165" s="12"/>
-      <c r="C165" s="14" t="s">
+      <c r="C165" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="D165" s="15"/>
-      <c r="E165" s="16"/>
+      <c r="D165" s="16"/>
+      <c r="E165" s="17"/>
     </row>
     <row r="166" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B166" s="9" t="s">
@@ -3856,11 +3883,11 @@
     </row>
     <row r="176" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B176" s="12"/>
-      <c r="C176" s="14" t="s">
+      <c r="C176" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="D176" s="15"/>
-      <c r="E176" s="16"/>
+      <c r="D176" s="16"/>
+      <c r="E176" s="17"/>
     </row>
     <row r="177" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B177" s="9" t="s">
@@ -4200,11 +4227,11 @@
     </row>
     <row r="201" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B201" s="12"/>
-      <c r="C201" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="D201" s="15"/>
-      <c r="E201" s="16"/>
+      <c r="C201" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D201" s="16"/>
+      <c r="E201" s="17"/>
     </row>
     <row r="202" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B202" s="9" t="s">
@@ -4217,7 +4244,7 @@
         <v>3</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
     <row r="203" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4231,7 +4258,7 @@
         <v>4</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="204" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4245,7 +4272,7 @@
         <v>8</v>
       </c>
       <c r="E204" s="6" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="205" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4259,7 +4286,7 @@
         <v>9</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="206" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4273,68 +4300,171 @@
         <v>10</v>
       </c>
       <c r="E206" s="6" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="207" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B207" s="12"/>
-      <c r="C207" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="D207" s="15"/>
-      <c r="E207" s="16"/>
+      <c r="B207" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C207" s="10">
+        <v>20</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E207" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="208" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B208" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="C208" s="10">
-        <v>20</v>
-      </c>
-      <c r="D208" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E208" s="6" t="s">
-        <v>247</v>
-      </c>
+      <c r="B208" s="12"/>
+      <c r="C208" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D208" s="16"/>
+      <c r="E208" s="17"/>
     </row>
     <row r="209" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="12"/>
-      <c r="C209" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="D209" s="15"/>
-      <c r="E209" s="16"/>
+      <c r="B209" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C209" s="10">
+        <v>21</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E209" s="6" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="210" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B210" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C210" s="10">
         <v>21</v>
       </c>
       <c r="D210" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E210" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="211" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B211" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C211" s="10">
+        <v>21</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E211" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="212" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B212" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C212" s="10">
+        <v>21</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E212" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="213" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B213" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C213" s="10">
+        <v>21</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E213" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="214" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B214" s="12"/>
+      <c r="C214" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D214" s="16"/>
+      <c r="E214" s="17"/>
+    </row>
+    <row r="215" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B215" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C215" s="10">
+        <v>22</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E215" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="216" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B216" s="12"/>
+      <c r="C216" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D216" s="16"/>
+      <c r="E216" s="17"/>
+    </row>
+    <row r="217" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B217" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C217" s="10">
+        <v>23</v>
+      </c>
+      <c r="D217" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E210" s="6" t="s">
+      <c r="E217" s="6" t="s">
         <v>264</v>
       </c>
     </row>
+    <row r="218" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B218" s="12"/>
+      <c r="C218" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="D218" s="16"/>
+      <c r="E218" s="17"/>
+    </row>
+    <row r="219" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B219" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C219" s="10">
+        <v>24</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E219" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C156:E156"/>
-    <mergeCell ref="C158:E158"/>
-    <mergeCell ref="C161:E161"/>
-    <mergeCell ref="C163:E163"/>
-    <mergeCell ref="C165:E165"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C209:E209"/>
+  <mergeCells count="27">
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C216:E216"/>
     <mergeCell ref="C154:E154"/>
     <mergeCell ref="C80:E80"/>
     <mergeCell ref="C90:E90"/>
@@ -4346,7 +4476,20 @@
     <mergeCell ref="C129:E129"/>
     <mergeCell ref="C115:E115"/>
     <mergeCell ref="C176:E176"/>
+    <mergeCell ref="C208:E208"/>
     <mergeCell ref="C201:E201"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C156:E156"/>
+    <mergeCell ref="C158:E158"/>
+    <mergeCell ref="C161:E161"/>
+    <mergeCell ref="C163:E163"/>
+    <mergeCell ref="C165:E165"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C68:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed an error with the voice lines folders. Added extra comments.
</commit_message>
<xml_diff>
--- a/voice_lines/Voice Lines Table.xlsx
+++ b/voice_lines/Voice Lines Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_Middlesex University\Third Year\PDE3400 Design Engineering Major Project\Development\audio processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_Middlesex University\Third Year\PDE3400 Design Engineering Major Project\_GitHub\AURI_Smartwatch_Software\voice_lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B5C685-510D-4745-B906-3B821A5A301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D452137B-8362-44C3-99CA-2AF51F3CCB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48225" yWindow="1425" windowWidth="25605" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53385" yWindow="780" windowWidth="23025" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="295">
   <si>
     <t>FOLDER</t>
   </si>
@@ -914,6 +914,12 @@
   </si>
   <si>
     <t>The heart rate is over 120BPM!</t>
+  </si>
+  <si>
+    <t>EXTRA WATCH</t>
+  </si>
+  <si>
+    <t>The watch is now charging!</t>
   </si>
 </sst>
 </file>
@@ -1252,11 +1258,8 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1264,8 +1267,11 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1565,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E219"/>
+  <dimension ref="B2:E221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E225" sqref="E225"/>
+    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E203" sqref="E203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1588,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1594,12 +1600,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
-      <c r="C4" s="16" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
@@ -2485,11 +2491,11 @@
     </row>
     <row r="68" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="13"/>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="17"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="16"/>
     </row>
     <row r="69" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="9" t="s">
@@ -2507,11 +2513,11 @@
     </row>
     <row r="70" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="13"/>
-      <c r="C70" s="16" t="s">
+      <c r="C70" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D70" s="16"/>
-      <c r="E70" s="17"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="16"/>
     </row>
     <row r="71" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="9" t="s">
@@ -2529,11 +2535,11 @@
     </row>
     <row r="72" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="13"/>
-      <c r="C72" s="16" t="s">
+      <c r="C72" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="17"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="16"/>
     </row>
     <row r="73" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="9" t="s">
@@ -2551,11 +2557,11 @@
     </row>
     <row r="74" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="12"/>
-      <c r="C74" s="18" t="s">
+      <c r="C74" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D74" s="16"/>
-      <c r="E74" s="17"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="16"/>
     </row>
     <row r="75" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="9" t="s">
@@ -2629,11 +2635,11 @@
     </row>
     <row r="80" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="12"/>
-      <c r="C80" s="18" t="s">
+      <c r="C80" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="16"/>
-      <c r="E80" s="17"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="16"/>
     </row>
     <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="9" t="s">
@@ -2919,11 +2925,11 @@
     </row>
     <row r="102" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="12"/>
-      <c r="C102" s="18" t="s">
+      <c r="C102" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D102" s="16"/>
-      <c r="E102" s="17"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="16"/>
     </row>
     <row r="103" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="9" t="s">
@@ -3011,11 +3017,11 @@
     </row>
     <row r="109" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="12"/>
-      <c r="C109" s="18" t="s">
+      <c r="C109" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D109" s="16"/>
-      <c r="E109" s="17"/>
+      <c r="D109" s="15"/>
+      <c r="E109" s="16"/>
     </row>
     <row r="110" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="9" t="s">
@@ -3089,11 +3095,11 @@
     </row>
     <row r="115" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="12"/>
-      <c r="C115" s="18" t="s">
+      <c r="C115" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D115" s="16"/>
-      <c r="E115" s="17"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="16"/>
     </row>
     <row r="116" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="9" t="s">
@@ -3611,11 +3617,11 @@
     </row>
     <row r="154" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B154" s="12"/>
-      <c r="C154" s="18" t="s">
+      <c r="C154" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="D154" s="16"/>
-      <c r="E154" s="17"/>
+      <c r="D154" s="15"/>
+      <c r="E154" s="16"/>
     </row>
     <row r="155" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="9" t="s">
@@ -3633,11 +3639,11 @@
     </row>
     <row r="156" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="12"/>
-      <c r="C156" s="18" t="s">
+      <c r="C156" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D156" s="16"/>
-      <c r="E156" s="17"/>
+      <c r="D156" s="15"/>
+      <c r="E156" s="16"/>
     </row>
     <row r="157" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="9" t="s">
@@ -3655,11 +3661,11 @@
     </row>
     <row r="158" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="12"/>
-      <c r="C158" s="18" t="s">
+      <c r="C158" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D158" s="16"/>
-      <c r="E158" s="17"/>
+      <c r="D158" s="15"/>
+      <c r="E158" s="16"/>
     </row>
     <row r="159" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B159" s="9" t="s">
@@ -3691,11 +3697,11 @@
     </row>
     <row r="161" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B161" s="12"/>
-      <c r="C161" s="18" t="s">
+      <c r="C161" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="D161" s="16"/>
-      <c r="E161" s="17"/>
+      <c r="D161" s="15"/>
+      <c r="E161" s="16"/>
     </row>
     <row r="162" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B162" s="9" t="s">
@@ -3713,11 +3719,11 @@
     </row>
     <row r="163" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B163" s="12"/>
-      <c r="C163" s="18" t="s">
+      <c r="C163" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="D163" s="16"/>
-      <c r="E163" s="17"/>
+      <c r="D163" s="15"/>
+      <c r="E163" s="16"/>
     </row>
     <row r="164" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B164" s="9" t="s">
@@ -3735,11 +3741,11 @@
     </row>
     <row r="165" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B165" s="12"/>
-      <c r="C165" s="18" t="s">
+      <c r="C165" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="D165" s="16"/>
-      <c r="E165" s="17"/>
+      <c r="D165" s="15"/>
+      <c r="E165" s="16"/>
     </row>
     <row r="166" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B166" s="9" t="s">
@@ -3883,11 +3889,11 @@
     </row>
     <row r="176" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B176" s="12"/>
-      <c r="C176" s="18" t="s">
+      <c r="C176" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="D176" s="16"/>
-      <c r="E176" s="17"/>
+      <c r="D176" s="15"/>
+      <c r="E176" s="16"/>
     </row>
     <row r="177" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B177" s="9" t="s">
@@ -4227,11 +4233,11 @@
     </row>
     <row r="201" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B201" s="12"/>
-      <c r="C201" s="18" t="s">
+      <c r="C201" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="D201" s="16"/>
-      <c r="E201" s="17"/>
+      <c r="D201" s="15"/>
+      <c r="E201" s="16"/>
     </row>
     <row r="202" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B202" s="9" t="s">
@@ -4319,11 +4325,11 @@
     </row>
     <row r="208" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B208" s="12"/>
-      <c r="C208" s="18" t="s">
+      <c r="C208" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="D208" s="16"/>
-      <c r="E208" s="17"/>
+      <c r="D208" s="15"/>
+      <c r="E208" s="16"/>
     </row>
     <row r="209" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B209" s="9" t="s">
@@ -4397,11 +4403,11 @@
     </row>
     <row r="214" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B214" s="12"/>
-      <c r="C214" s="18" t="s">
+      <c r="C214" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="D214" s="16"/>
-      <c r="E214" s="17"/>
+      <c r="D214" s="15"/>
+      <c r="E214" s="16"/>
     </row>
     <row r="215" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B215" s="9" t="s">
@@ -4419,11 +4425,11 @@
     </row>
     <row r="216" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B216" s="12"/>
-      <c r="C216" s="18" t="s">
+      <c r="C216" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="D216" s="16"/>
-      <c r="E216" s="17"/>
+      <c r="D216" s="15"/>
+      <c r="E216" s="16"/>
     </row>
     <row r="217" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B217" s="9" t="s">
@@ -4441,15 +4447,15 @@
     </row>
     <row r="218" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B218" s="12"/>
-      <c r="C218" s="18" t="s">
+      <c r="C218" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="D218" s="16"/>
-      <c r="E218" s="17"/>
+      <c r="D218" s="15"/>
+      <c r="E218" s="16"/>
     </row>
     <row r="219" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B219" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C219" s="10">
         <v>24</v>
@@ -4461,23 +4467,43 @@
         <v>292</v>
       </c>
     </row>
+    <row r="220" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B220" s="12"/>
+      <c r="C220" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="D220" s="15"/>
+      <c r="E220" s="16"/>
+    </row>
+    <row r="221" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B221" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C221" s="10">
+        <v>25</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E221" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C216:E216"/>
-    <mergeCell ref="C154:E154"/>
+  <mergeCells count="28">
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C201:E201"/>
+    <mergeCell ref="C136:E136"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="C176:E176"/>
     <mergeCell ref="C80:E80"/>
     <mergeCell ref="C90:E90"/>
     <mergeCell ref="C98:E98"/>
     <mergeCell ref="C102:E102"/>
     <mergeCell ref="C109:E109"/>
-    <mergeCell ref="C136:E136"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="C176:E176"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C201:E201"/>
+    <mergeCell ref="C220:E220"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C214:E214"/>
@@ -4490,6 +4516,9 @@
     <mergeCell ref="C72:E72"/>
     <mergeCell ref="C70:E70"/>
     <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C216:E216"/>
+    <mergeCell ref="C154:E154"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>